<commit_message>
Comentarios generales ejercicio 5 - P2
</commit_message>
<xml_diff>
--- a/TP1/portada_lanacion.xlsx
+++ b/TP1/portada_lanacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A306"/>
+  <dimension ref="A1:A297"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//clima/</t>
+          <t>https://www.lanacion.com.ar/clima/</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//</t>
+          <t>https://www.lanacion.com.ar/</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/#</t>
+          <t>https://www.lanacion.com.ar#</t>
         </is>
       </c>
     </row>
@@ -653,7 +653,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/</t>
+          <t>https://www.lanacion.com.ar/autos/</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/</t>
+          <t>https://www.lanacion.com.ar/salud/</t>
         </is>
       </c>
     </row>
@@ -1003,21 +1003,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//juegos/</t>
+          <t>https://www.lanacion.com.ar/juegos/</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//suscriptores/</t>
+          <t>https://www.lanacion.com.ar/suscriptores/</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//mis-notas/</t>
+          <t>https://www.lanacion.com.ar/mis-notas/</t>
         </is>
       </c>
     </row>
@@ -1066,1510 +1066,1447 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//opinion/la-casta-que-rodea-al-presidente-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/el-papelon-de-lula-da-silva-la-burla-de-maduro-y-el-camino-hacia-ningun-lado-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/el-pacto-no-escrito-entre-javier-milei-y-cristina-kirchner-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/edmundo-gonzalez-urrutia-llego-a-espana-que-le-otorgo-asilo-politico-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/el-papelon-de-lula-da-silva-la-burla-de-maduro-y-el-camino-hacia-ningun-lado-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/la-casta-que-rodea-al-presidente-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/edmundo-gonzalez-urrutia-llego-a-espana-que-le-otorgo-asilo-politico-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/politica/el-pacto-no-escrito-entre-javier-milei-y-cristina-kirchner-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/internaron-al-jefe-de-gabinete-guillermo-francos-por-un-cuadro-gastrointestinal-agudo-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/politica/internaron-al-jefe-de-gabinete-guillermo-francos-por-un-cuadro-gastrointestinal-agudo-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/oriente-medio-un-argentino-fue-asesinado-en-un-ataque-terrorista-donde-murieron-otros-dos-civiles-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/oriente-medio-un-argentino-fue-asesinado-en-un-ataque-terrorista-donde-murieron-otros-dos-civiles-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/dolar/dolar-hoy-dolar-blue-hoy-a-cuanto-cotiza-este-domingo-8-de-septiembre-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/lionel-scaloni-sorprendio-con-una-reflexion-acerca-de-su-referente-como-entrenador-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/edmundo-gonzalez-urrutia-llego-a-espana-que-le-otorgo-asilo-politico-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/rugby/julian-montoya-tuvo-su-tarde-sonada-el-capitan-llego-a-su-partido-100-en-los-pumas-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/la-jugada-del-arquero-de-penarol-que-desato-un-escandalo-tres-expulsados-y-seis-amonestados-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/seguridad/una-turista-italiana-denuncio-que-fue-agredida-sexualmente-en-los-esteros-del-ibera-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/tenis/argentina-en-las-finales-de-la-copa-davis-2024-dias-horarios-tv-y-como-ver-online-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/seguridad/un-policia-murio-tras-recibir-una-patada-en-la-espalda-cuando-vecinos-defendieron-a-un-delincuente-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/oriente-medio-un-argentino-fue-asesinado-en-un-ataque-terrorista-donde-murieron-otros-dos-civiles-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/atletismo/el-increible-accidente-de-la-paratleta-italiana-que-perdio-la-medalla-dorada-y-conmovio-a-todos-en-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/atletismo/el-increible-accidente-de-la-paratleta-italiana-que-perdio-la-medalla-dorada-y-conmovio-a-todos-en-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/fuerte-discusion-entre-el-presidente-de-talleres-y-andres-merlos-ingreso-al-vestuario-con-armas-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/copa-argentina-un-boca-surrealista-con-un-gol-que-no-debio-ser-22-penales-y-un-entrenador-cargado-de-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/sociedad/me-enseno-a-posicionar-mi-negocio-el-fuerte-impacto-de-un-programa-educativo-gratuito-y-con-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/rugby/julian-montoya-tuvo-su-tarde-sonada-el-capitan-llego-a-su-partido-100-en-los-pumas-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/politica/la-denuncia-contra-el-camarista-hornos-recalo-en-comodoro-py-y-hay-preocupacion-en-casacion-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/el-click-politico-que-cristina-kirchner-le-reclama-al-peronismo-para-enfrentar-a-milei-y-sus-aliados-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/hija-de-una-argentina-la-foto-que-delato-la-relacion-entre-el-principe-felipe-e-isabel-sartorius-el-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/al-volante/los-autos-con-motores-turbo-chicos-siguen-creciendo-que-modelos-los-ofrecen-y-por-que-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/el-padre-guillermo-furlong-rescato-las-observaciones-de-charles-darwin-sobre-los-gauchos-argentinos-nid18052024/</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/fuerte-discusion-entre-el-presidente-de-talleres-y-andres-merlos-ingreso-al-vestuario-con-armas-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/politica/siento-verguenza-fabiola-yanez-busca-retomar-la-ofensiva-con-chats-en-los-que-fernandez-aceptaria-su-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/quien-es-el-agente-inmobiliario-y-principal-sospechoso-de-enviar-un-paquete-explosivo-a-nicolas-pino-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/economia/para-que-importar-para-poder-exportar-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/cara-de-lloriquear-nuevos-chats-revelan-discusiones-en-el-gobierno-de-alberto-fernandez-por-el-rol-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/milei-mas-rapido-que-kirchner-para-atacar-a-la-prensa-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/la-denuncia-contra-el-camarista-hornos-recalo-en-comodoro-py-y-hay-preocupacion-en-casacion-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/conversaciones-de-domingo/dante-sica-el-programa-de-desregulaciones-de-milei-es-similar-al-de-macri-pero-macri-fue-un-liberal-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/hija-de-una-argentina-la-foto-que-delato-la-relacion-entre-el-principe-felipe-e-isabel-sartorius-el-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/economia/las-contradicciones-del-gobierno-juegan-en-contra-de-bajar-el-riesgo-pais-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/el-padre-guillermo-furlong-rescato-las-observaciones-de-charles-darwin-sobre-los-gauchos-argentinos-nid18052024/</t>
+          <t>https://www.lanacion.com.ar/deportes/</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/el-gobierno-rechaza-la-decision-de-maduro-de-quitarle-a-brasil-la-custodia-de-la-embajada-argentina-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/un-ataque-de-locura-el-poder-de-fuego-de-la-seleccion-argentina-va-mas-alla-de-messi-y-scaloni-lo-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/venezuela-busca-quitar-a-brasil-la-custodia-de-la-embajada-argentina-en-caracas-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/boca-juniors/el-particular-festejo-de-diego-martinez-tras-la-victoria-de-boca-ante-talleres-y-la-explicacion-del-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/quienes-son-los-opositores-que-se-refugian-en-la-embajada-argentina-en-caracas-y-como-se-vive-el-nid27032024/</t>
+          <t>https://www.lanacion.com.ar/deportes/rugby/tucumanazo-en-santa-fe-mateo-carreras-fue-la-figura-frente-a-australia-y-tomas-albornoz-hizo-brillar-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/siento-verguenza-fabiola-yanez-busca-retomar-la-ofensiva-con-chats-en-los-que-fernandez-aceptaria-su-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/pacho-odonnell-el-edadismo-su-adiccion-a-la-gimnasia-su-regreso-a-los-escenarios-y-por-que-hay-que-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/para-que-importar-para-poder-exportar-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/hallaron-muerto-a-james-hollcroft-actor-de-televisa-que-estaba-desaparecido-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//opinion/milei-mas-rapido-que-kirchner-para-atacar-a-la-prensa-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/la-jugada-del-arquero-de-penarol-que-desato-un-escandalo-tres-expulsados-y-seis-amonestados-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//conversaciones-de-domingo/dante-sica-el-programa-de-desregulaciones-de-milei-es-similar-al-de-macri-pero-macri-fue-un-liberal-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/dibu-martinez-mostro-lo-que-come-el-plantel-de-la-seleccion-argentina-y-sorprendio-a-todos-que-me-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/las-contradicciones-del-gobierno-juegan-en-contra-de-bajar-el-riesgo-pais-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/martinez-sosa-cobro-comisiones-de-200-mil-polizas-optativas-con-una-trampa-en-gendarmeria-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/</t>
+          <t>https://www.lanacion.com.ar/seguridad/adn-del-crimen-confirman-la-condena-para-el-poderoso-juez-que-era-la-pieza-clave-de-la-banda-formada-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/un-ataque-de-locura-el-poder-de-fuego-de-la-seleccion-argentina-va-mas-alla-de-messi-y-scaloni-lo-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/inversiones/la-zona-impensada-en-donde-los-alquileres-dejan-la-renta-mas-alta-del-mercado-10-en-dolares-nid28082024/</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/boca-juniors/el-particular-festejo-de-diego-martinez-tras-la-victoria-de-boca-ante-talleres-y-la-explicacion-del-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/autos/al-volante/los-autos-con-motores-turbo-chicos-siguen-creciendo-que-modelos-los-ofrecen-y-por-que-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/rugby/tucumanazo-en-santa-fe-mateo-carreras-fue-la-figura-frente-a-australia-y-tomas-albornoz-hizo-brillar-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/musica/waldo-de-los-rios-el-genio-musical-que-cumpliria-90-anos-sus-frustraciones-un-auto-incendiado-y-el-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/personajes/pacho-odonnell-el-edadismo-su-adiccion-a-la-gimnasia-su-regreso-a-los-escenarios-y-por-que-hay-que-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/el-papa-cumplio-su-promesa-de-visitar-a-misioneros-argentinos-que-trabajan-en-la-periferia-de-la-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/hallaron-muerto-a-james-hollcroft-actor-de-televisa-que-estaba-desaparecido-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/politica/quien-es-el-agente-inmobiliario-y-principal-sospechoso-de-enviar-un-paquete-explosivo-a-nicolas-pino-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/la-jugada-del-arquero-de-penarol-que-desato-un-escandalo-tres-expulsados-y-seis-amonestados-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/kathleen-booth-la-precursora-de-las-redes-neuronales-que-hace-casi-80-anos-nos-enseno-a-hablar-con-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/quien-es-el-autor-de-la-famosa-frase-aquellos-que-no-pueden-recordar-el-pasado-estan-condenados-a-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/la-fascinante-experiencia-de-viajar-junto-con-el-papa-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/martinez-sosa-cobro-comisiones-de-200-mil-polizas-optativas-con-una-trampa-en-gendarmeria-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/estados-unidos/torre-hertz-asi-fue-la-implosion-del-edificio-abandonado-de-22-pisos-en-luisiana-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//seguridad/adn-del-crimen-confirman-la-condena-para-el-poderoso-juez-que-era-la-pieza-clave-de-la-banda-formada-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/jair-bolsonaro-mostro-su-poder-de-movilizacion-con-una-marcha-multitudinaria-y-pidio-el-juicio-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/todo-lo-que-un-aviso-inmobiliario-debe-evitar-en-la-publicacion-si-se-quiere-vender-la-propiedad-a-nid29082024/</t>
+          <t xml:space="preserve">https://lnmas.lanacion.com.ar/ </t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/mente/prevenir-el-alzheimer-los-habitos-que-ayudan-a-evitar-la-enfermedad-nid08092024/</t>
+          <t xml:space="preserve">https://lnmas.lanacion.com.ar/ </t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/musica/waldo-de-los-rios-el-genio-musical-que-cumpliria-90-anos-sus-frustraciones-un-auto-incendiado-y-el-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/politica/el-inquietante-retorno-de-la-violencia-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/el-papa-cumplio-su-promesa-de-visitar-a-misioneros-argentinos-que-trabajan-en-la-periferia-de-la-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/inmuebles-comerciales/locales-cuanto-cuesta-alquilar-en-palermo-soho-y-la-avenida-alvear-y-cual-es-la-zona-mas-cara-nid27082024/</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/personajes/martin-fierro-2024-una-noche-agridulce-con-muchas-estrellas-pero-tambien-con-varias-ausencias-y-un-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/a-12-anos-de-la-muerte-de-su-hija-blanca-benjamin-vicuna-la-recordo-con-un-emotivo-video-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//tecnologia/kathleen-booth-la-precursora-de-las-redes-neuronales-que-hace-casi-80-anos-nos-enseno-a-hablar-con-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/martin-fierro-2024-una-noche-agridulce-con-muchas-estrellas-pero-tambien-con-varias-ausencias-y-un-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//opinion/la-fascinante-experiencia-de-viajar-junto-con-el-papa-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/anto-roccuzzo-acompano-a-su-hijo-al-entrenamiento-y-quedo-impactada-ante-la-presencia-de-un-animal-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//estados-unidos/torre-hertz-asi-fue-la-implosion-del-edificio-abandonado-de-22-pisos-en-luisiana-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/ideas/el-futuro-del-trabajo-hasta-donde-la-inteligencia-artificial-revolucionara-la-empresa-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/jair-bolsonaro-mostro-su-poder-de-movilizacion-con-una-marcha-multitudinaria-y-pidio-el-juicio-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/juegos/</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://lnmas.lanacion.com.ar/ </t>
+          <t>https://www.lanacion.com.ar/juegos/sopa-de-letras/</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://lnmas.lanacion.com.ar/ </t>
+          <t>https://www.lanacion.com.ar/juegos/trivias/test-de-interes-general-contesta-las-10-preguntas-de-la-semana-sobre-la-avalancha-en-bariloche-la-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/el-inquietante-retorno-de-la-violencia-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/juegos/crucimini/</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/inmuebles-comerciales/locales-cuanto-cuesta-alquilar-en-palermo-soho-y-la-avenida-alvear-y-cual-es-la-zona-mas-cara-nid27082024/</t>
+          <t>https://www.lanacion.com.ar/juegos/palabra-oculta/</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/a-12-anos-de-la-muerte-de-su-hija-blanca-benjamin-vicuna-la-recordo-con-un-emotivo-video-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/el-emotivo-adios-de-mirtha-legrand-a-selva-aleman-era-un-ser-adorable-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sociedad/salud-identifican-cinco-formas-de-envejecer-gracias-a-los-datos-de-50000-escaneres-cerebrales-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/maxima-en-buenos-aires-la-intimidad-de-la-fiesta-de-cumpleanos-80-de-su-madre-en-el-yatch-club-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//revista-living/centro-de-doble-altura-vistas-interiores-y-jardin-envolvente-la-formula-de-una-casa-llena-de-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/franco-colapinto-reacciono-cuando-la-china-suarez-lo-empezo-a-seguir-y-despues-se-arrepintio-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//ideas/el-futuro-del-trabajo-hasta-donde-la-inteligencia-artificial-revolucionara-la-empresa-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/television/los-detalles-del-regreso-de-susana-a-la-tv-grabo-un-sketch-con-caro-pardiaco-y-entrevisto-a-rodrigo-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/</t>
+          <t>https://foodit.lanacion.com.ar/</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//juegos/sopa-de-letras/</t>
+          <t>https://foodit.lanacion.com.ar/novedades-y-tendencias/</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//juegos/trivias/test-de-interes-general-contesta-las-10-preguntas-de-la-semana-sobre-la-avalancha-en-bariloche-la-nid08092024/</t>
+          <t>https://foodit.lanacion.com.ar/guias-de-cocina/</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//juegos/crucimini/</t>
+          <t>https://foodit.lanacion.com.ar/masterclass/</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//juegos/palabra-oculta/</t>
+          <t>https://suscripciones.lanacion.com.ar/suscripcion/V/3?cv=800&amp;fc=831</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/personajes/el-emotivo-adios-de-mirtha-legrand-a-selva-aleman-era-un-ser-adorable-nid07092024/</t>
+          <t>https://foodit.lanacion.com.ar/</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/maxima-en-buenos-aires-la-intimidad-de-la-fiesta-de-cumpleanos-80-de-su-madre-en-el-yatch-club-nid06092024/</t>
+          <t>https://suscripciones.lanacion.com.ar/suscripcion/V/3?cv=800&amp;fc=831</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/franco-colapinto-reacciono-cuando-la-china-suarez-lo-empezo-a-seguir-y-despues-se-arrepintio-nid06092024/</t>
+          <t>https://foodit.lanacion.com.ar/novedades-y-tendencias/menu-de-almuerzos-y-cenas-para-optimizar-el-rendimiento-fisico-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/television/los-detalles-del-regreso-de-susana-a-la-tv-grabo-un-sketch-con-caro-pardiaco-y-entrevisto-a-rodrigo-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/suscriptores/</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>https://foodit.lanacion.com.ar/</t>
+          <t>https://www.lanacion.com.ar/tema/la-nacion-cerca/</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>https://foodit.lanacion.com.ar/novedades-y-tendencias/</t>
+          <t>https://newsletter.lanacion.com.ar/</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>https://foodit.lanacion.com.ar/guias-de-cocina/</t>
+          <t>https://www.lanacion.com.ar/opinion/carta-de-suscriptores/</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>https://foodit.lanacion.com.ar/masterclass/</t>
+          <t>https://suscripciones.lanacion.com.ar/suscripcion/E/1/1/</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>https://suscripciones.lanacion.com.ar/suscripcion/V/3?cv=800&amp;fc=831</t>
+          <t>https://www.lanacion.com.ar/sabado/un-clasico-de-la-parrilla-julio-iglesias-mandaba-un-avion-para-hacerse-llevar-los-bifes-a-brasil-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>https://foodit.lanacion.com.ar/</t>
+          <t>https://www.lanacion.com.ar/juegos/trivias/trivia-exclusiva-cuanto-sabes-sobre-la-guerra-de-los-treinta-anos-nid04092024/</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>https://suscripciones.lanacion.com.ar/suscripcion/V/3?cv=800&amp;fc=831</t>
+          <t>https://www.lanacion.com.ar/revista-jardin/10-cosas-que-no-sabias-sobre-las-piletas-biologicas-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>https://foodit.lanacion.com.ar/novedades-y-tendencias/menu-de-almuerzos-y-cenas-para-optimizar-el-rendimiento-fisico-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/negocios/el-local-argentino-que-impuso-las-medialunas-en-una-capital-gastronomica-mundial-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/suscriptores/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/dia-del-productor-agropecuario-maneja-7300-hectareas-y-cuenta-la-formula-de-un-impactante-logro-en-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tema/la-nacion-cerca/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/un-lujo-lleno-el-tanque-de-la-camioneta-y-se-quedo-atonico-por-lo-que-tuvo-que-pagar-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>https://newsletter.lanacion.com.ar/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/como-hace-el-hornero-para-construir-su-nido-en-no-mas-de-15-dias-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//opinion/carta-de-suscriptores/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/ramon-diaz-el-refugio-rural-desde-donde-una-de-las-glorias-de-river-planea-otra-vida-y-habla-sin-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>https://suscripciones.lanacion.com.ar/suscripcion/E/1/1/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sabado/un-clasico-de-la-parrilla-julio-iglesias-mandaba-un-avion-para-hacerse-llevar-los-bifes-a-brasil-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/asi-se-veria-campanita-en-la-vida-real-segun-la-inteligencia-artificial-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//juegos/trivias/trivia-exclusiva-cuanto-sabes-sobre-la-guerra-de-los-treinta-anos-nid04092024/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/las-cinco-carreras-que-nadie-elige-para-estudiar-en-la-argentina-segun-la-inteligencia-artificial-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//revista-jardin/10-cosas-que-no-sabias-sobre-las-piletas-biologicas-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/juegos-paralimpicos-de-paris-2024-google-le-dedico-su-doodle-a-la-ceremonia-de-clausura-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/negocios/el-local-argentino-que-impuso-las-medialunas-en-una-capital-gastronomica-mundial-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/dia-del-productor-agropecuario-maneja-7300-hectareas-y-cuenta-la-formula-de-un-impactante-logro-en-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/un-libertario-esclavo-de-sus-promesas-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/un-lujo-lleno-el-tanque-de-la-camioneta-y-se-quedo-atonico-por-lo-que-tuvo-que-pagar-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/la-logica-del-reality-invadio-a-la-politica-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/como-hace-el-hornero-para-construir-su-nido-en-no-mas-de-15-dias-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/llego-el-mes-de-la-alergia-a-la-realidad-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/ramon-diaz-el-refugio-rural-desde-donde-una-de-las-glorias-de-river-planea-otra-vida-y-habla-sin-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/editoriales/</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/</t>
+          <t>https://www.lanacion.com.ar/editoriales/el-desafio-de-construir-un-estado-decente-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//tecnologia/asi-se-veria-campanita-en-la-vida-real-segun-la-inteligencia-artificial-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/editoriales/juntos-y-arremangados-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//tecnologia/las-cinco-carreras-que-nadie-elige-para-estudiar-en-la-argentina-segun-la-inteligencia-artificial-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/ahora-se-que-no-soy-un-hombre-de-exito-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//tecnologia/juegos-paralimpicos-de-paris-2024-google-le-dedico-su-doodle-a-la-ceremonia-de-clausura-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/horoscopo/horoscopo-las-predicciones-de-jimena-la-torre-para-la-semana-del-8-al-14-de-septiembre-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/opinion/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/en-las-redes/tras-volverse-viral-en-espana-en-argentina-ya-se-puede-buscar-pareja-en-el-supermercado-cual-es-la-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//opinion/un-libertario-esclavo-de-sus-promesas-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/que-se-sabe-de-la-muerte-de-james-hollcroft-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//opinion/la-logica-del-reality-invadio-a-la-politica-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/cuidado-cuerpo-belleza/la-bebida-que-se-recomienda-tomar-antes-de-dormir-para-prevenir-calambres-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//opinion/llego-el-mes-de-la-alergia-a-la-realidad-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/loterias/ganaron-mas-de-1230-millones-en-el-quini-6-cuales-fueron-los-numeros-de-la-suerte-del-sorteo-del-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/editoriales/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/mascotas/un-dato-revelador-desmiente-una-creencia-popular-sobre-los-gatos-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//editoriales/el-desafio-de-construir-un-estado-decente-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/en-las-redes/enumero-los-gastos-fijos-que-tuvo-con-su-pareja-en-agosto-y-se-hizo-viral-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//editoriales/juntos-y-arremangados-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/copa-argentina-un-boca-surrealista-con-un-gol-que-no-debio-ser-22-penales-y-un-entrenador-cargado-de-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//opinion/ahora-se-que-no-soy-un-hombre-de-exito-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/la-jugada-del-arquero-de-penarol-que-desato-un-escandalo-tres-expulsados-y-seis-amonestados-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/en-las-redes/tras-volverse-viral-en-espana-en-argentina-ya-se-puede-buscar-pareja-en-el-supermercado-cual-es-la-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/el-papa-cumplio-su-promesa-de-visitar-a-misioneros-argentinos-que-trabajan-en-la-periferia-de-la-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//ciencia/estas-son-las-impactantes-predicciones-del-cientifico-carl-sagan-que-ya-comenzaron-a-cumplirse-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/atletismo/el-increible-accidente-de-la-paratleta-italiana-que-perdio-la-medalla-dorada-y-conmovio-a-todos-en-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/cuidado-cuerpo-belleza/la-bebida-que-se-recomienda-tomar-antes-de-dormir-para-prevenir-calambres-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/pacho-odonnell-el-edadismo-su-adiccion-a-la-gimnasia-su-regreso-a-los-escenarios-y-por-que-hay-que-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sociedad/natividad-de-la-santisima-virgen-maria-su-historia-y-que-oracion-rezar-para-pedir-su-ayuda-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/jugaron-en-grande-el-historico-triunfo-de-los-pumas-frente-a-los-wallabies-en-una-jornada-repleta-de-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//loterias/ganaron-mas-de-1230-millones-en-el-quini-6-cuales-fueron-los-numeros-de-la-suerte-del-sorteo-del-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//feriados/2024/11-de-septiembre-el-dia-del-maestro-es-feriado-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/polo/polo-los-cambiaso-ya-no-son-dos-sino-tres-pero-camilo-castagnola-pudo-con-todos-y-gano-el-abierto-de-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/en-las-redes/enumero-los-gastos-fijos-que-tuvo-con-su-pareja-en-agosto-y-se-hizo-viral-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/economia/</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sociedad/de-que-murio-melina-furman-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/dolar-hoy/</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/cara-de-lloriquear-nuevos-chats-revelan-discusiones-en-el-gobierno-de-alberto-fernandez-por-el-rol-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/economia/indices/</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/la-denuncia-contra-el-camarista-hornos-recalo-en-comodoro-py-y-hay-preocupacion-en-casacion-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/personajes/pacho-odonnell-el-edadismo-su-adiccion-a-la-gimnasia-su-regreso-a-los-escenarios-y-por-que-hay-que-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/negocios/</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/rugby/tucumanazo-en-santa-fe-mateo-carreras-fue-la-figura-frente-a-australia-y-tomas-albornoz-hizo-brillar-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/tema/emprendedores-tid53673/</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/san-fernando-como-paso-de-ser-una-localidad-poco-buscada-de-zona-norte-a-atraer-grandes-inversiones-nid31082024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/</t>
+          <t>https://www.lanacion.com.ar/economia/los-motores-que-aceleran-el-despliegue-de-la-nueva-economia-de-la-introversion-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/polo/polo-los-cambiaso-ya-no-son-dos-sino-tres-pero-camilo-castagnola-pudo-con-todos-y-gano-el-abierto-de-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/economia/jubilaciones-que-paso-con-el-poder-adquisitivo-de-los-haberes-en-lo-que-va-de-este-ano-nid02092024/</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/</t>
+          <t>https://www.lanacion.com.ar/economia/las-claves-del-blanqueo-segun-las-ultimas-aclaraciones-reglamentarias-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/dolar-hoy/</t>
+          <t>https://www.lanacion.com.ar/economia/finanzas-los-cambios-recientes-en-la-industria-de-fondos-comunes-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/indices/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/cine/asi-cerro-el-festival-de-venecia-de-la-alegria-de-pedro-almodovar-a-la-dolorosa-ausencia-de-nicole-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/negocios/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/television/los-detalles-del-regreso-de-susana-a-la-tv-grabo-un-sketch-con-caro-pardiaco-y-entrevisto-a-rodrigo-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tema/emprendedores-tid53673/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/musica/a-dos-anos-de-la-muerte-de-marciano-cantero-su-hijo-javier-edita-uno-de-los-albumes-ineditos-que-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/</t>
+          <t>https://www.lanacion.com.ar/salud/</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/los-motores-que-aceleran-el-despliegue-de-la-nueva-economia-de-la-introversion-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/salud/vida_sana/</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/jubilaciones-que-paso-con-el-poder-adquisitivo-de-los-haberes-en-lo-que-va-de-este-ano-nid02092024/</t>
+          <t>https://www.lanacion.com.ar/salud/nutricion/</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/las-claves-del-blanqueo-segun-las-ultimas-aclaraciones-reglamentarias-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/salud/fitness/</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/finanzas-los-cambios-recientes-en-la-industria-de-fondos-comunes-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/salud/mente/</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/</t>
+          <t>https://www.lanacion.com.ar/salud/descanso/</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/cine/asi-cerro-el-festival-de-venecia-de-la-alegria-de-pedro-almodovar-a-la-dolorosa-ausencia-de-nicole-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/turismo/viajes/</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/musica/el-nuevo-album-de-david-gilmour-entre-la-finitud-el-trabajo-en-familia-y-el-infaltable-toque-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/salud/el-mercado-de-los-sabores-exoticos-y-otros-platos-para-paladares-exigentes-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/television/rituales-maquillaje-y-zozobra-como-se-vive-un-partido-de-la-seleccion-desde-una-cabina-de-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/salud/5-ejercicios-simples-para-aliviar-el-dolor-de-espalda-y-cuello-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/</t>
+          <t>https://www.lanacion.com.ar/salud/por-que-conectamos-mas-con-las-criticas-que-con-los-elogios-y-repetimos-conductas-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/vida_sana/</t>
+          <t>https://www.lanacion.com.ar/salud/nutricion/oro-blanco-el-probiotico-natural-perfecto-para-aumentar-las-defensas-y-mejorar-el-estado-de-animo-nid03092024/</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/nutricion/</t>
+          <t>https://www.lanacion.com.ar/autos/</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/fitness/</t>
+          <t>https://www.lanacion.com.ar/autos/tendencias/</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/mente/</t>
+          <t>https://www.lanacion.com.ar/autos/test-drive/</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/descanso/</t>
+          <t>https://www.lanacion.com.ar/autos/electricos/</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//turismo/viajes/</t>
+          <t>https://www.lanacion.com.ar/autos/cuanto-cuesta-la-ford-ranger-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/el-mercado-de-los-sabores-exoticos-y-otros-platos-para-paladares-exigentes-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/autos/cuanto-cuestan-las-pick-ups-en-septiembre-luego-de-la-baja-de-precios-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/5-ejercicios-simples-para-aliviar-el-dolor-de-espalda-y-cuello-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/autos/las-motos-se-suman-a-la-baja-de-precios-cuales-son-los-modelos-que-retrocedieron-en-septiembre-nid04092024/</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/por-que-conectamos-mas-con-las-criticas-que-con-los-elogios-y-repetimos-conductas-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/autos/cuanto-cuesta-el-toyota-corolla-cross-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//salud/nutricion/oro-blanco-el-probiotico-natural-perfecto-para-aumentar-las-defensas-y-mejorar-el-estado-de-animo-nid03092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/tendencias/</t>
+          <t>https://www.lanacion.com.ar/propiedades/construccion-y-diseno/</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/test-drive/</t>
+          <t>https://www.lanacion.com.ar/propiedades/inmuebles-comerciales/</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/electricos/</t>
+          <t>https://www.lanacion.com.ar/propiedades/inversiones/</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/cuanto-cuesta-la-ford-ranger-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/historias-es-argentino-compro-un-burdel-para-crear-un-corredor-en-zona-norte-y-hara-un-cable-carril-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/cuanto-cuestan-las-pick-ups-en-septiembre-luego-de-la-baja-de-precios-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/el-barrio-verde-que-vive-un-boom-de-construccion-y-tiene-hasta-dos-proyectos-en-una-misma-cuadra-nid02092024/</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/las-motos-se-suman-a-la-baja-de-precios-cuales-son-los-modelos-que-retrocedieron-en-septiembre-nid04092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/construccion-y-diseno/historias-es-argentino-se-anticipo-a-un-megaproyecto-petrolero-y-desarrollo-la-ciudad-que-potenciara-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/cuanto-cuesta-el-toyota-corolla-cross-en-septiembre-2024-luego-de-la-baja-del-impuesto-pais-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/la-ciudad-de-nueva-york-que-paga-us9000-por-mudarse-cuales-son-los-requisitos-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/</t>
+          <t>https://lncampo.lanacion.com.ar/remates</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/construccion-y-diseno/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/agricultura/</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/inmuebles-comerciales/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/ganaderia/</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/inversiones/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/tecnologias/</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/historias-es-argentino-compro-un-burdel-para-crear-un-corredor-en-zona-norte-y-hara-un-cable-carril-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/regionales/</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/el-barrio-verde-que-vive-un-boom-de-construccion-y-tiene-hasta-dos-proyectos-en-una-misma-cuadra-nid02092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/estupor-frente-a-un-grave-atentado-y-los-avances-de-la-desregulacion-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/construccion-y-diseno/historias-es-argentino-se-anticipo-a-un-megaproyecto-petrolero-y-desarrollo-la-ciudad-que-potenciara-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/agricultura/el-repunte-del-maiz-y-de-la-soja-en-chicago-se-mira-pero-no-se-copia-en-el-mercado-argentino-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//propiedades/casas-y-departamentos/la-ciudad-de-nueva-york-que-paga-us9000-por-mudarse-cuales-son-los-requisitos-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/mas-papistas-que-el-papa-fuerte-malestar-entre-productores-por-una-marcha-atras-del-gobierno-con-una-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/no-nos-van-a-callar-el-presidente-de-la-rural-califico-al-atentado-de-un-episodio-de-una-argentina-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>https://lncampo.lanacion.com.ar/remates</t>
+          <t>https://www.lanacion.com.ar/lifestyle/</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/agricultura/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/controlaba-las-piletas-de-un-completo-cuando-noto-algo-extrano-que-flotaba-estaba-helada-e-inmovil-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/ganaderia/</t>
+          <t>https://www.lanacion.com.ar/sabado/un-clasico-de-la-parrilla-julio-iglesias-mandaba-un-avion-para-hacerse-llevar-los-bifes-a-brasil-nid07092024/</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/tecnologias/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/que-es-la-gente-nutritiva-y-cuales-son-sus-caracteristicas-nid17112023/</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/regionales/</t>
+          <t>https://www.lanacion.com.ar/revista-living/conoce-la-casa-de-la-influencer-coty-crotto-nid06092024/</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/estupor-frente-a-un-grave-atentado-y-los-avances-de-la-desregulacion-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/revista-living/visitamos-la-casa-estudio-de-dos-creadores-de-objetos-de-diseno-con-inspiracion-marplatense-nid05092024/</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/agricultura/el-repunte-del-maiz-y-de-la-soja-en-chicago-se-mira-pero-no-se-copia-en-el-mercado-argentino-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/sociedad/natividad-de-la-santisima-virgen-maria-su-historia-y-que-oracion-rezar-para-pedir-su-ayuda-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/mas-papistas-que-el-papa-fuerte-malestar-entre-productores-por-una-marcha-atras-del-gobierno-con-una-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/feriados/2024/11-de-septiembre-el-dia-del-maestro-es-feriado-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/campo/no-nos-van-a-callar-el-presidente-de-la-rural-califico-al-atentado-de-un-episodio-de-una-argentina-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/economia/jubilados-anses-fijo-el-haber-maximo-a-partir-de-septiembre-en-cuanto-queda-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/</t>
+          <t>https://www.lanacion.com.ar/loterias/quini-6-cual-es-el-premio-para-el-sorteo-de-este-domingo-8-de-septiembre-nid08092024/</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/controlaba-las-piletas-de-un-completo-cuando-noto-algo-extrano-que-flotaba-estaba-helada-e-inmovil-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sabado/un-clasico-de-la-parrilla-julio-iglesias-mandaba-un-avion-para-hacerse-llevar-los-bifes-a-brasil-nid07092024/</t>
+          <t>https://www.lanacion.com.ar/ultimas-noticias/</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//lifestyle/que-es-la-gente-nutritiva-y-cuales-son-sus-caracteristicas-nid17112023/</t>
+          <t>https://www.lanacion.com.ar/politica/</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//revista-living/conoce-la-casa-de-la-influencer-coty-crotto-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/economia/</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//revista-living/visitamos-la-casa-estudio-de-dos-creadores-de-objetos-de-diseno-con-inspiracion-marplatense-nid05092024/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//sociedad/dia-internacional-del-periodista-por-que-se-celebra-hoy-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/sociedad/</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/en-que-hotel-es-la-ceremonia-de-los-martin-fierro-2024-nid06092024/</t>
+          <t>https://www.lanacion.com.ar/opinion/</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/jubilados-anses-fijo-el-haber-maximo-a-partir-de-septiembre-en-cuanto-queda-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/deportes/</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//loterias/quini-6-cual-es-el-premio-para-el-sorteo-de-este-domingo-8-de-septiembre-nid08092024/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/ultimas-noticias/</t>
+          <t>https://edicionimpresa.lanacion.com.ar/la-nacion?_ga=2.226421138.948268382.1669638459-1845108145.1619557251/</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/</t>
+          <t>https://lnmas.lanacion.com.ar/</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/</t>
+          <t>https://club.lanacion.com.ar/</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/</t>
+          <t>https://www.somosohlala.com/</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sociedad/</t>
+          <t>https://www.lanacion.com.ar/revista-hola/</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/opinion/</t>
+          <t>https://www.lanacion.com.ar/revista-living/</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/</t>
+          <t>https://www.lanacion.com.ar/revista-jardin/</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/</t>
+          <t>https://www.lanacion.com.ar/revista-lugares/</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/</t>
+          <t>https://es.rollingstone.com/arg/</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>https://edicionimpresa.lanacion.com.ar/la-nacion?_ga=2.226421138.948268382.1669638459-1845108145.1619557251/</t>
+          <t>https://bonvivir.com/</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>https://lnmas.lanacion.com.ar/</t>
+          <t>https://colecciones.lanacion.com.ar</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>https://club.lanacion.com.ar/</t>
+          <t>https://www.utdt.edu/ver_contenido.php?id_contenido=1111&amp;id_item_menu=2327</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>https://www.somosohlala.com/</t>
+          <t>https://fundacionlanacion.org.ar/</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-hola/</t>
+          <t>https://www.lanacion.com.ar/mapa-del-sitio/</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-living/</t>
+          <t>https://www.contacto.lanacion.com.ar/ayuda?_ga=2.125953413.948268382.1669638459-1845108145.1619557251</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-jardin/</t>
+          <t>https://club.lanacion.com.ar/ayuda/</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-lugares/</t>
+          <t>https://www.contacto.lanacion.com.ar/tyc?_ga=2.125953413.948268382.1669638459-1845108145.1619557251/</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>https://es.rollingstone.com/arg/</t>
+          <t>https://www.lanacion.in/</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>https://bonvivir.com/</t>
+          <t>https://suscripciones.lanacion.com.ar/suscribirme?_ga=2.159335858.948268382.1669638459-1845108145.1619557251/</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>https://colecciones.lanacion.com.ar</t>
+          <t>https://www.facebook.com/lanacion</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>https://www.utdt.edu/ver_contenido.php?id_contenido=1111&amp;id_item_menu=2327</t>
+          <t>https://twitter.com/LANACION</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>https://fundacionlanacion.org.ar/</t>
+          <t>https://www.instagram.com/lanacioncom/</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/mapa-del-sitio/</t>
+          <t>https://www.lanacion.com.ar/arc/outboundfeeds/rss/?outputType=xml</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>https://www.contacto.lanacion.com.ar/ayuda?_ga=2.125953413.948268382.1669638459-1845108145.1619557251</t>
+          <t>https://play.google.com/store/apps/details?id=app.lanacion.activity&amp;hl=es_419&amp;pli=1</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>https://club.lanacion.com.ar/ayuda/</t>
+          <t>https://apps.apple.com/ar/app/la-nacion/id410689702</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>https://www.contacto.lanacion.com.ar/tyc?_ga=2.125953413.948268382.1669638459-1845108145.1619557251/</t>
+          <t>https://policies.google.com/terms?hl=es-419</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>https://www.lanacion.in/</t>
+          <t>https://policies.google.com/privacy?hl=es-419</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>https://suscripciones.lanacion.com.ar/suscribirme?_ga=2.159335858.948268382.1669638459-1845108145.1619557251/</t>
+          <t>https://www.gda.com/</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/lanacion</t>
-        </is>
-      </c>
-    </row>
-    <row r="298">
-      <c r="A298" t="inlineStr">
-        <is>
-          <t>https://twitter.com/LANACION</t>
-        </is>
-      </c>
-    </row>
-    <row r="299">
-      <c r="A299" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/lanacioncom/</t>
-        </is>
-      </c>
-    </row>
-    <row r="300">
-      <c r="A300" t="inlineStr">
-        <is>
-          <t>https://www.lanacion.com.ar/arc/outboundfeeds/rss/?outputType=xml</t>
-        </is>
-      </c>
-    </row>
-    <row r="301">
-      <c r="A301" t="inlineStr">
-        <is>
-          <t>https://play.google.com/store/apps/details?id=app.lanacion.activity&amp;hl=es_419&amp;pli=1</t>
-        </is>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" t="inlineStr">
-        <is>
-          <t>https://apps.apple.com/ar/app/la-nacion/id410689702</t>
-        </is>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" t="inlineStr">
-        <is>
-          <t>https://policies.google.com/terms?hl=es-419</t>
-        </is>
-      </c>
-    </row>
-    <row r="304">
-      <c r="A304" t="inlineStr">
-        <is>
-          <t>https://policies.google.com/privacy?hl=es-419</t>
-        </is>
-      </c>
-    </row>
-    <row r="305">
-      <c r="A305" t="inlineStr">
-        <is>
-          <t>https://www.gda.com/</t>
-        </is>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306" t="inlineStr">
         <is>
           <t>http://qr.afip.gob.ar/?qr=HJMakbCpenWNdXYfqXtEDQ,,</t>
         </is>

</xml_diff>